<commit_message>
Committing changes to TrueAug_SymDiGCN_CiteSeer_output.xlsx
</commit_message>
<xml_diff>
--- a/TrueAug_SymDiGCN_CiteSeer_output.xlsx
+++ b/TrueAug_SymDiGCN_CiteSeer_output.xlsx
@@ -843,7 +843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A494"/>
+  <dimension ref="A1:A503"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -861,3449 +861,3512 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Epoch:492, time:9.665039, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:501, time:9.649806, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Epoch:491, time:9.731945, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:500, time:9.438108, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Epoch:490, time:9.546413, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:499, time:9.327127, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Epoch:489, time:10.181904, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:498, time:9.611853, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Epoch:488, time:9.823899, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:497, time:9.535737, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Epoch:487, time:9.978501, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:496, time:9.260726, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Epoch:486, time:9.788491, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:495, time:14.170702, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Epoch:485, time:9.561090, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:494, time:9.904561, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Epoch:484, time:9.588706, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:493, time:9.826703, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Epoch:483, time:10.354257, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:492, time:9.665039, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Epoch:482, time:9.990207, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:491, time:9.731945, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Epoch:481, time:11.382630, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:490, time:9.546413, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Epoch:480, time:10.691122, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:489, time:10.181904, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Epoch:479, time:10.639102, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:488, time:9.823899, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Epoch:478, time:13.291723, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:487, time:9.978501, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Epoch:477, time:11.393646, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:486, time:9.788491, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Epoch:476, time:10.782908, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:485, time:9.561090, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Epoch:475, time:10.658318, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:484, time:9.588706, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Epoch:474, time:11.061198, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:483, time:10.354257, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Epoch:473, time:15.223918, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:482, time:9.990207, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Epoch:472, time:17.417031, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:481, time:11.382630, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Epoch:471, time:17.246876, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:480, time:10.691122, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Epoch:470, time:17.694973, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:479, time:10.639102, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Epoch:469, time:17.849216, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:478, time:13.291723, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Epoch:468, time:18.136074, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:477, time:11.393646, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Epoch:467, time:9.345089, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:476, time:10.782908, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Epoch:466, time:10.312622, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:475, time:10.658318, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Epoch:465, time:9.531579, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:474, time:11.061198, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Epoch:464, time:9.522034, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:473, time:15.223918, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Epoch:463, time:9.634985, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:472, time:17.417031, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Epoch:462, time:9.608490, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:471, time:17.246876, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Epoch:461, time:9.608213, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:470, time:17.694973, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Epoch:460, time:9.758211, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:469, time:17.849216, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Epoch:459, time:9.540488, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:468, time:18.136074, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Epoch:458, time:10.112104, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:467, time:9.345089, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Epoch:457, time:9.670007, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:466, time:10.312622, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Epoch:456, time:9.593237, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:465, time:9.531579, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Epoch:455, time:9.469584, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:464, time:9.522034, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Epoch:454, time:9.650097, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:463, time:9.634985, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Epoch:453, time:9.502644, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:462, time:9.608490, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Epoch:452, time:9.528419, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:461, time:9.608213, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Epoch:451, time:9.534432, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:460, time:9.758211, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Epoch:450, time:9.523595, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:459, time:9.540488, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Epoch:449, time:9.545942, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:458, time:10.112104, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Epoch:448, time:9.449264, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:457, time:9.670007, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Epoch:447, time:9.645727, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:456, time:9.593237, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Epoch:446, time:10.475939, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:455, time:9.469584, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Epoch:445, time:10.531253, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:454, time:9.650097, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Epoch:444, time:9.920135, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:453, time:9.502644, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Epoch:443, time:9.337900, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:452, time:9.528419, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Epoch:442, time:9.281134, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:451, time:9.534432, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Epoch:441, time:9.471284, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:450, time:9.523595, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Epoch:440, time:9.261921, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:449, time:9.545942, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Epoch:439, time:9.347075, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:448, time:9.449264, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Epoch:438, time:9.383788, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:447, time:9.645727, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Epoch:437, time:9.314226, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:446, time:10.475939, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Epoch:436, time:9.350935, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:445, time:10.531253, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Epoch:435, time:9.456839, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:444, time:9.920135, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Epoch:434, time:9.312558, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:443, time:9.337900, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Epoch:433, time:9.235655, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:442, time:9.281134, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Epoch:432, time:9.042333, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:441, time:9.471284, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Epoch:431, time:9.444113, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:440, time:9.261921, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Epoch:430, time:9.375131, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:439, time:9.347075, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Epoch:429, time:9.385804, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:438, time:9.383788, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Epoch:428, time:9.188344, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:437, time:9.314226, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Epoch:427, time:9.346066, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:436, time:9.350935, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Epoch:426, time:9.420545, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:435, time:9.456839, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Epoch:425, time:9.315494, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:434, time:9.312558, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Epoch:424, time:8.930940, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:433, time:9.235655, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Epoch:423, time:9.097773, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:432, time:9.042333, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Epoch:422, time:9.463205, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:431, time:9.444113, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Epoch:421, time:9.446325, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:430, time:9.375131, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Epoch:420, time:9.473701, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:429, time:9.385804, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Epoch:419, time:9.260526, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:428, time:9.188344, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Epoch:418, time:9.247035, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:427, time:9.346066, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Epoch:417, time:9.228128, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:426, time:9.420545, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Epoch:416, time:9.317154, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:425, time:9.315494, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Epoch:415, time:10.478542, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:424, time:8.930940, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Epoch:414, time:10.252038, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:423, time:9.097773, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Epoch:413, time:10.604662, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:422, time:9.463205, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Epoch:412, time:9.631000, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:421, time:9.446325, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Epoch:411, time:10.535891, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:420, time:9.473701, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Epoch:410, time:10.571866, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:419, time:9.260526, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Epoch:409, time:10.548386, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:418, time:9.247035, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Epoch:408, time:10.453052, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:417, time:9.228128, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Epoch:407, time:10.003239, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:416, time:9.317154, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Epoch:406, time:10.252537, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:415, time:10.478542, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Epoch:405, time:10.554522, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:414, time:10.252038, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Epoch:404, time:9.506900, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:413, time:10.604662, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Epoch:403, time:9.462647, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:412, time:9.631000, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Epoch:402, time:9.282170, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:411, time:10.535891, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Epoch:401, time:9.259573, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:410, time:10.571866, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Epoch:400, time:9.819477, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:409, time:10.548386, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Epoch:399, time:10.650677, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:408, time:10.453052, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Epoch:398, time:10.705105, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:407, time:10.003239, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Epoch:397, time:10.453674, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:406, time:10.252537, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Epoch:396, time:10.297158, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:405, time:10.554522, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Epoch:395, time:10.660311, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:404, time:9.506900, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Epoch:394, time:10.401362, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:403, time:9.462647, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Epoch:393, time:10.300137, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:402, time:9.282170, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Epoch:392, time:9.330457, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:401, time:9.259573, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Epoch:391, time:9.030211, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:400, time:9.819477, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Epoch:390, time:9.443750, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:399, time:10.650677, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Epoch:389, time:9.584098, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:398, time:10.705105, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Epoch:388, time:9.676791, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:397, time:10.453674, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Epoch:387, time:9.149655, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:396, time:10.297158, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Epoch:386, time:9.403090, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:395, time:10.660311, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Epoch:385, time:9.383082, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:394, time:10.401362, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Epoch:384, time:9.505402, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:393, time:10.300137, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Epoch:383, time:9.355801, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:392, time:9.330457, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Epoch:382, time:9.517281, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:391, time:9.030211, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Epoch:381, time:9.391339, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:390, time:9.443750, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Epoch:380, time:10.384428, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:389, time:9.584098, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Epoch:379, time:10.372850, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:388, time:9.676791, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Epoch:378, time:9.545491, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:387, time:9.149655, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Epoch:377, time:9.415490, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:386, time:9.403090, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Epoch:376, time:9.545512, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:385, time:9.383082, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Epoch:375, time:9.588542, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:384, time:9.505402, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Epoch:374, time:10.149606, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:383, time:9.355801, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Epoch:373, time:9.577385, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:382, time:9.517281, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Epoch:372, time:9.749693, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:381, time:9.391339, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Epoch:371, time:9.438760, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:380, time:10.384428, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Epoch:370, time:10.154187, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:379, time:10.372850, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Epoch:369, time:9.584223, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:378, time:9.545491, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Epoch:368, time:9.942912, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:377, time:9.415490, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Epoch:367, time:10.152066, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:376, time:9.545512, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Epoch:366, time:9.495063, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:375, time:9.588542, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Epoch:365, time:9.383113, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:374, time:10.149606, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Epoch:364, time:9.439770, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:373, time:9.577385, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Epoch:363, time:9.732389, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:372, time:9.749693, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Epoch:362, time:10.038732, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:371, time:9.438760, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Epoch:361, time:9.297659, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:370, time:10.154187, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Epoch:360, time:9.336353, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:369, time:9.584223, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Epoch:359, time:9.313357, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:368, time:9.942912, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Epoch:358, time:10.365083, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:367, time:10.152066, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Epoch:357, time:10.112669, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:366, time:9.495063, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Epoch:356, time:9.887265, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:365, time:9.383113, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Epoch:355, time:9.539761, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:364, time:9.439770, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Epoch:354, time:9.962208, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:363, time:9.732389, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Epoch:353, time:9.329243, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:362, time:10.038732, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Epoch:352, time:9.361496, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:361, time:9.297659, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Epoch:351, time:9.413660, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:360, time:9.336353, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Epoch:350, time:9.418414, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:359, time:9.313357, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Epoch:349, time:9.412924, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:358, time:10.365083, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Epoch:348, time:9.348671, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:357, time:10.112669, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Epoch:347, time:9.331747, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:356, time:9.887265, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Epoch:346, time:9.407916, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:355, time:9.539761, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Epoch:345, time:9.376490, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:354, time:9.962208, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Epoch:344, time:9.416188, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:353, time:9.329243, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Epoch:343, time:9.311254, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:352, time:9.361496, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Epoch:342, time:10.152397, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:351, time:9.413660, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Epoch:341, time:9.860352, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:350, time:9.418414, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Epoch:340, time:10.058972, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:349, time:9.412924, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Epoch:339, time:9.900698, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:348, time:9.348671, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Epoch:338, time:10.043228, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:347, time:9.331747, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Epoch:337, time:9.259761, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:346, time:9.407916, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Epoch:336, time:9.284558, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:345, time:9.376490, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Epoch:335, time:9.244012, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:344, time:9.416188, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Epoch:334, time:9.422040, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:343, time:9.311254, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Epoch:333, time:9.222349, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:342, time:10.152397, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Epoch:332, time:9.429449, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:341, time:9.860352, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Epoch:331, time:9.355216, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:340, time:10.058972, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Epoch:330, time:9.297462, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:339, time:9.900698, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Epoch:329, time:9.329894, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:338, time:10.043228, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Epoch:328, time:9.667214, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:337, time:9.259761, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Epoch:327, time:9.531332, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:336, time:9.284558, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Epoch:326, time:9.318629, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:335, time:9.244012, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Epoch:325, time:9.224811, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:334, time:9.422040, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Epoch:324, time:9.263304, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:333, time:9.222349, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Epoch:323, time:9.167589, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:332, time:9.429449, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Epoch:322, time:9.273779, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:331, time:9.355216, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Epoch:321, time:9.216713, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:330, time:9.297462, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Epoch:320, time:9.234457, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:329, time:9.329894, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Epoch:319, time:9.184377, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:328, time:9.667214, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Epoch:318, time:9.306207, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:327, time:9.531332, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Epoch:317, time:9.130543, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:326, time:9.318629, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Epoch:316, time:9.735495, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:325, time:9.224811, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Epoch:315, time:9.319167, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:324, time:9.263304, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Epoch:314, time:9.301131, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:323, time:9.167589, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Epoch:313, time:9.314152, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:322, time:9.273779, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Epoch:312, time:9.358135, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:321, time:9.216713, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Epoch:311, time:9.655780, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:320, time:9.234457, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Epoch:310, time:9.319532, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:319, time:9.184377, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Epoch:309, time:9.344337, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:318, time:9.306207, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Epoch:308, time:9.311820, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:317, time:9.130543, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Epoch:307, time:9.237505, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:316, time:9.735495, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Epoch:306, time:9.505077, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:315, time:9.319167, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Epoch:305, time:10.206166, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:314, time:9.301131, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Epoch:304, time:10.359485, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:313, time:9.314152, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Epoch:303, time:9.791240, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:312, time:9.358135, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Epoch:302, time:10.053333, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:311, time:9.655780, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Epoch:301, time:10.267582, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:310, time:9.319532, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Epoch:300, time:10.219019, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:309, time:9.344337, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Epoch:299, time:9.332254, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:308, time:9.311820, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Epoch:298, time:9.099087, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:307, time:9.237505, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Epoch:297, time:9.617158, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:306, time:9.505077, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Epoch:296, time:9.634429, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:305, time:10.206166, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Epoch:295, time:9.312654, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:304, time:10.359485, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Epoch:294, time:9.117365, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:303, time:9.791240, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Epoch:293, time:9.102996, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:302, time:10.053333, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Epoch:292, time:10.091643, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:301, time:10.267582, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Epoch:291, time:9.703962, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:300, time:10.219019, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Epoch:290, time:9.395289, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:299, time:9.332254, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Epoch:289, time:9.260391, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:298, time:9.099087, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Epoch:288, time:9.273844, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:297, time:9.617158, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Epoch:287, time:9.191228, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:296, time:9.634429, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Epoch:286, time:9.247929, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:295, time:9.312654, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Epoch:285, time:9.641901, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:294, time:9.117365, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Epoch:284, time:9.224030, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:293, time:9.102996, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Epoch:283, time:9.374810, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:292, time:10.091643, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Epoch:282, time:10.322654, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:291, time:9.703962, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Epoch:281, time:10.124052, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:290, time:9.395289, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Epoch:280, time:9.634297, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:289, time:9.260391, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Epoch:279, time:9.573686, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:288, time:9.273844, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Epoch:278, time:9.798080, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:287, time:9.191228, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Epoch:277, time:9.520572, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:286, time:9.247929, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Epoch:276, time:9.597568, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:285, time:9.641901, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Epoch:275, time:9.443286, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:284, time:9.224030, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Epoch:274, time:9.389261, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:283, time:9.374810, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Epoch:273, time:9.555876, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:282, time:10.322654, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Epoch:272, time:9.488961, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:281, time:10.124052, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Epoch:271, time:9.393395, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:280, time:9.634297, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Epoch:270, time:9.920826, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:279, time:9.573686, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Epoch:269, time:9.941875, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:278, time:9.798080, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Epoch:268, time:14.006636, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:277, time:9.520572, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Epoch:267, time:11.945849, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:276, time:9.597568, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Epoch:266, time:11.276525, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:275, time:9.443286, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Epoch:265, time:10.611570, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:274, time:9.389261, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Epoch:264, time:12.138474, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:273, time:9.555876, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Epoch:263, time:10.615481, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:272, time:9.488961, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Epoch:262, time:11.948614, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:271, time:9.393395, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Epoch:261, time:13.045376, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:270, time:9.920826, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Epoch:260, time:16.643257, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:269, time:9.941875, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Epoch:259, time:23.159261, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:268, time:14.006636, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Epoch:258, time:24.138797, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:267, time:11.945849, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Epoch:257, time:17.597739, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:266, time:11.276525, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Epoch:256, time:15.121541, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:265, time:10.611570, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Epoch:255, time:10.173377, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:264, time:12.138474, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Epoch:254, time:13.901095, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:263, time:10.615481, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Epoch:253, time:12.831509, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:262, time:11.948614, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Epoch:252, time:9.743743, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:261, time:13.045376, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Epoch:251, time:10.609293, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:260, time:16.643257, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Epoch:250, time:9.919076, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:259, time:23.159261, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Epoch:249, time:10.032958, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:258, time:24.138797, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Epoch:248, time:9.752469, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:257, time:17.597739, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Epoch:247, time:9.636446, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:256, time:15.121541, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Epoch:246, time:10.250260, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:255, time:10.173377, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Epoch:245, time:10.510076, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:254, time:13.901095, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Epoch:244, time:9.467415, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:253, time:12.831509, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Epoch:243, time:9.545637, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:252, time:9.743743, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Epoch:242, time:10.343339, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:251, time:10.609293, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Epoch:241, time:11.635263, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:250, time:9.919076, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Epoch:240, time:12.197394, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:249, time:10.032958, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Epoch:239, time:11.231335, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:248, time:9.752469, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Epoch:238, time:10.700053, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:247, time:9.636446, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Epoch:237, time:10.826342, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:246, time:10.250260, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Epoch:236, time:10.730981, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:245, time:10.510076, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Epoch:235, time:10.688308, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:244, time:9.467415, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Epoch:234, time:10.660731, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:243, time:9.545637, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Epoch:233, time:10.851370, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:242, time:10.343339, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Epoch:232, time:13.746957, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:241, time:11.635263, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Epoch:231, time:16.825635, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:240, time:12.197394, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Epoch:230, time:18.110029, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:239, time:11.231335, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Epoch:229, time:28.500070, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:238, time:10.700053, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Epoch:228, time:11.413636, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:237, time:10.826342, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Epoch:227, time:9.114116, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:236, time:10.730981, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Epoch:226, time:8.536223, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:235, time:10.688308, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Epoch:225, time:9.360809, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:234, time:10.660731, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Epoch:224, time:10.146283, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:233, time:10.851370, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Epoch:223, time:9.297108, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:232, time:13.746957, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Epoch:222, time:8.917316, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:231, time:16.825635, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Epoch:221, time:9.719652, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:230, time:18.110029, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Epoch:220, time:11.306098, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:229, time:28.500070, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Epoch:219, time:9.037593, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:228, time:11.413636, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>Epoch:218, time:11.409882, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:227, time:9.114116, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>Epoch:217, time:9.015418, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:226, time:8.536223, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>Epoch:216, time:9.132804, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:225, time:9.360809, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>Epoch:215, time:9.644043, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:224, time:10.146283, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>Epoch:214, time:9.226883, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:223, time:9.297108, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>Epoch:213, time:8.894328, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:222, time:8.917316, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>Epoch:212, time:9.013119, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:221, time:9.719652, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Epoch:211, time:9.791013, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:220, time:11.306098, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>Epoch:210, time:9.275434, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:219, time:9.037593, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Epoch:209, time:9.035873, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:218, time:11.409882, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Epoch:208, time:8.854391, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:217, time:9.015418, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>Epoch:207, time:8.932319, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:216, time:9.132804, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Epoch:206, time:9.059160, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:215, time:9.644043, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Epoch:205, time:9.455591, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:214, time:9.226883, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Epoch:204, time:9.851263, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:213, time:8.894328, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Epoch:203, time:9.758970, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:212, time:9.013119, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>Epoch:202, time:9.905586, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:211, time:9.791013, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>Epoch:201, time:9.898726, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:210, time:9.275434, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>Epoch:200, time:9.285792, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:209, time:9.035873, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>Epoch:199, time:9.524733, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:208, time:8.854391, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>Epoch:198, time:11.620375, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:207, time:8.932319, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>Epoch:197, time:9.047408, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:206, time:9.059160, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>Epoch:196, time:8.914351, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:205, time:9.455591, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>Epoch:195, time:8.922461, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:204, time:9.851263, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>Epoch:194, time:9.459258, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:203, time:9.758970, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>Epoch:193, time:9.568551, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:202, time:9.905586, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>Epoch:192, time:9.184635, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:201, time:9.898726, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>Epoch:191, time:9.934530, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:200, time:9.285792, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>Epoch:190, time:9.920578, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:199, time:9.524733, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>Epoch:189, time:9.486984, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:198, time:11.620375, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Epoch:188, time:9.824769, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:197, time:9.047408, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>Epoch:187, time:9.117601, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:196, time:8.914351, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>Epoch:186, time:9.067031, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:195, time:8.922461, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>Epoch:185, time:10.767168, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:194, time:9.459258, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>Epoch:184, time:10.886015, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:193, time:9.568551, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>Epoch:183, time:11.739977, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:192, time:9.184635, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>Epoch:182, time:10.969228, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:191, time:9.934530, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>Epoch:181, time:11.279598, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:190, time:9.920578, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>Epoch:180, time:10.841132, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:189, time:9.486984, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>Epoch:179, time:10.709636, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:188, time:9.824769, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>Epoch:178, time:11.234958, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:187, time:9.117601, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>Epoch:177, time:11.134071, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:186, time:9.067031, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>Epoch:176, time:11.449718, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:185, time:10.767168, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Epoch:175, time:10.992860, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:184, time:10.886015, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>Epoch:174, time:10.961991, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:183, time:11.739977, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>Epoch:173, time:11.114695, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:182, time:10.969228, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>Epoch:172, time:11.412684, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:181, time:11.279598, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>Epoch:171, time:11.229661, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:180, time:10.841132, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>Epoch:170, time:11.507543, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:179, time:10.709636, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>Epoch:169, time:11.475435, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:178, time:11.234958, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>Epoch:168, time:11.379001, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:177, time:11.134071, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>Epoch:167, time:11.733441, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:176, time:11.449718, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>Epoch:166, time:11.081132, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:175, time:10.992860, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>Epoch:165, time:11.381860, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:174, time:10.961991, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>Epoch:164, time:11.565470, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:173, time:11.114695, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>Epoch:163, time:10.850779, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:172, time:11.412684, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>Epoch:162, time:11.330768, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:171, time:11.229661, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>Epoch:161, time:10.644356, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:170, time:11.507543, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>Epoch:160, time:11.351932, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:169, time:11.475435, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>Epoch:159, time:10.884506, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:168, time:11.379001, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>Epoch:158, time:12.090905, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:167, time:11.733441, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>Epoch:157, time:11.851535, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:166, time:11.081132, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>Epoch:156, time:11.880067, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:165, time:11.381860, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>Epoch:155, time:10.591366, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:164, time:11.565470, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>Epoch:154, time:11.032485, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:163, time:10.850779, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>Epoch:153, time:11.572792, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:162, time:11.330768, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>Epoch:152, time:10.727026, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:161, time:10.644356, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>Epoch:151, time:11.135508, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:160, time:11.351932, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>Epoch:150, time:11.498559, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:159, time:10.884506, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>Epoch:149, time:11.815126, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:158, time:12.090905, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>Epoch:148, time:11.233013, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:157, time:11.851535, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>Epoch:147, time:11.326096, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:156, time:11.880067, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>Epoch:146, time:11.833452, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:155, time:10.591366, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>Epoch:145, time:10.876513, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:154, time:11.032485, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>Epoch:144, time:11.448502, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:153, time:11.572792, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>Epoch:143, time:11.240492, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:152, time:10.727026, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>Epoch:142, time:10.456415, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:151, time:11.135508, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>Epoch:141, time:10.676594, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:150, time:11.498559, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>Epoch:140, time:11.277915, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:149, time:11.815126, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>Epoch:139, time:10.588472, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:148, time:11.233013, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>Epoch:138, time:10.757246, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:147, time:11.326096, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>Epoch:137, time:10.655624, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
+          <t>Epoch:146, time:11.833452, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>Epoch:136, time:11.273646, test_Acc: 37.10, test_bacc: 32.65, test_f1: 24.69</t>
+          <t>Epoch:145, time:10.876513, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>Epoch:135, time:11.867645, test_Acc: 37.10, test_bacc: 32.65, test_f1: 24.69</t>
+          <t>Epoch:144, time:11.448502, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>Epoch:134, time:11.616587, test_Acc: 37.10, test_bacc: 32.65, test_f1: 24.69</t>
+          <t>Epoch:143, time:11.240492, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>Epoch:133, time:11.547907, test_Acc: 37.10, test_bacc: 32.65, test_f1: 24.69</t>
+          <t>Epoch:142, time:10.456415, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>Epoch:132, time:10.880928, test_Acc: 35.30, test_bacc: 31.45, test_f1: 23.53</t>
+          <t>Epoch:141, time:10.676594, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>Epoch:131, time:11.420415, test_Acc: 35.30, test_bacc: 31.45, test_f1: 23.53</t>
+          <t>Epoch:140, time:11.277915, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>Epoch:130, time:11.089761, test_Acc: 35.20, test_bacc: 31.51, test_f1: 23.40</t>
+          <t>Epoch:139, time:10.588472, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>Epoch:129, time:10.386480, test_Acc: 35.20, test_bacc: 31.51, test_f1: 23.40</t>
+          <t>Epoch:138, time:10.757246, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>Epoch:128, time:11.016525, test_Acc: 34.50, test_bacc: 31.01, test_f1: 22.87</t>
+          <t>Epoch:137, time:10.655624, test_Acc: 38.30, test_bacc: 33.49, test_f1: 25.53</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>Epoch:127, time:11.471888, test_Acc: 34.50, test_bacc: 31.01, test_f1: 22.87</t>
+          <t>Epoch:136, time:11.273646, test_Acc: 37.10, test_bacc: 32.65, test_f1: 24.69</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>Epoch:126, time:11.029035, test_Acc: 33.70, test_bacc: 30.49, test_f1: 22.21</t>
+          <t>Epoch:135, time:11.867645, test_Acc: 37.10, test_bacc: 32.65, test_f1: 24.69</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>Epoch:125, time:12.505707, test_Acc: 33.70, test_bacc: 30.49, test_f1: 22.21</t>
+          <t>Epoch:134, time:11.616587, test_Acc: 37.10, test_bacc: 32.65, test_f1: 24.69</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>Epoch:124, time:11.311944, test_Acc: 33.40, test_bacc: 30.39, test_f1: 21.89</t>
+          <t>Epoch:133, time:11.547907, test_Acc: 37.10, test_bacc: 32.65, test_f1: 24.69</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>Epoch:123, time:11.772120, test_Acc: 33.40, test_bacc: 30.39, test_f1: 21.89</t>
+          <t>Epoch:132, time:10.880928, test_Acc: 35.30, test_bacc: 31.45, test_f1: 23.53</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>Epoch:122, time:11.114527, test_Acc: 33.40, test_bacc: 30.39, test_f1: 21.89</t>
+          <t>Epoch:131, time:11.420415, test_Acc: 35.30, test_bacc: 31.45, test_f1: 23.53</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>Epoch:121, time:11.740549, test_Acc: 33.40, test_bacc: 30.39, test_f1: 21.89</t>
+          <t>Epoch:130, time:11.089761, test_Acc: 35.20, test_bacc: 31.51, test_f1: 23.40</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>Epoch:120, time:11.097250, test_Acc: 31.80, test_bacc: 29.18, test_f1: 20.76</t>
+          <t>Epoch:129, time:10.386480, test_Acc: 35.20, test_bacc: 31.51, test_f1: 23.40</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>Epoch:119, time:11.125878, test_Acc: 31.80, test_bacc: 29.18, test_f1: 20.76</t>
+          <t>Epoch:128, time:11.016525, test_Acc: 34.50, test_bacc: 31.01, test_f1: 22.87</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>Epoch:118, time:11.128359, test_Acc: 31.20, test_bacc: 28.77, test_f1: 20.21</t>
+          <t>Epoch:127, time:11.471888, test_Acc: 34.50, test_bacc: 31.01, test_f1: 22.87</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>Epoch:117, time:12.309861, test_Acc: 31.20, test_bacc: 28.77, test_f1: 20.21</t>
+          <t>Epoch:126, time:11.029035, test_Acc: 33.70, test_bacc: 30.49, test_f1: 22.21</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>Epoch:116, time:10.919320, test_Acc: 30.80, test_bacc: 28.71, test_f1: 19.40</t>
+          <t>Epoch:125, time:12.505707, test_Acc: 33.70, test_bacc: 30.49, test_f1: 22.21</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>Epoch:115, time:11.382323, test_Acc: 30.80, test_bacc: 28.71, test_f1: 19.40</t>
+          <t>Epoch:124, time:11.311944, test_Acc: 33.40, test_bacc: 30.39, test_f1: 21.89</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>Epoch:114, time:11.001650, test_Acc: 30.40, test_bacc: 28.43, test_f1: 19.05</t>
+          <t>Epoch:123, time:11.772120, test_Acc: 33.40, test_bacc: 30.39, test_f1: 21.89</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>Epoch:113, time:11.391892, test_Acc: 30.40, test_bacc: 28.43, test_f1: 19.05</t>
+          <t>Epoch:122, time:11.114527, test_Acc: 33.40, test_bacc: 30.39, test_f1: 21.89</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>Epoch:112, time:10.759627, test_Acc: 30.20, test_bacc: 28.33, test_f1: 18.79</t>
+          <t>Epoch:121, time:11.740549, test_Acc: 33.40, test_bacc: 30.39, test_f1: 21.89</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>Epoch:111, time:11.819430, test_Acc: 30.20, test_bacc: 28.33, test_f1: 18.79</t>
+          <t>Epoch:120, time:11.097250, test_Acc: 31.80, test_bacc: 29.18, test_f1: 20.76</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>Epoch:110, time:11.440632, test_Acc: 30.00, test_bacc: 28.30, test_f1: 18.00</t>
+          <t>Epoch:119, time:11.125878, test_Acc: 31.80, test_bacc: 29.18, test_f1: 20.76</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>Epoch:109, time:11.945087, test_Acc: 30.00, test_bacc: 28.30, test_f1: 18.00</t>
+          <t>Epoch:118, time:11.128359, test_Acc: 31.20, test_bacc: 28.77, test_f1: 20.21</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>Epoch:108, time:11.341464, test_Acc: 30.00, test_bacc: 28.30, test_f1: 18.00</t>
+          <t>Epoch:117, time:12.309861, test_Acc: 31.20, test_bacc: 28.77, test_f1: 20.21</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>Epoch:107, time:11.205988, test_Acc: 30.00, test_bacc: 28.30, test_f1: 18.00</t>
+          <t>Epoch:116, time:10.919320, test_Acc: 30.80, test_bacc: 28.71, test_f1: 19.40</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>Epoch:106, time:11.058895, test_Acc: 29.90, test_bacc: 28.25, test_f1: 17.60</t>
+          <t>Epoch:115, time:11.382323, test_Acc: 30.80, test_bacc: 28.71, test_f1: 19.40</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>Epoch:105, time:11.460838, test_Acc: 29.90, test_bacc: 28.25, test_f1: 17.60</t>
+          <t>Epoch:114, time:11.001650, test_Acc: 30.40, test_bacc: 28.43, test_f1: 19.05</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>Epoch:104, time:11.180882, test_Acc: 29.90, test_bacc: 28.25, test_f1: 17.60</t>
+          <t>Epoch:113, time:11.391892, test_Acc: 30.40, test_bacc: 28.43, test_f1: 19.05</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>Epoch:103, time:10.792564, test_Acc: 29.90, test_bacc: 28.25, test_f1: 17.60</t>
+          <t>Epoch:112, time:10.759627, test_Acc: 30.20, test_bacc: 28.33, test_f1: 18.79</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>Epoch:102, time:11.128788, test_Acc: 29.80, test_bacc: 28.15, test_f1: 17.64</t>
+          <t>Epoch:111, time:11.819430, test_Acc: 30.20, test_bacc: 28.33, test_f1: 18.79</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>Epoch:101, time:13.083462, test_Acc: 29.80, test_bacc: 28.15, test_f1: 17.64</t>
+          <t>Epoch:110, time:11.440632, test_Acc: 30.00, test_bacc: 28.30, test_f1: 18.00</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>Epoch:100, time:11.609606, test_Acc: 29.40, test_bacc: 27.83, test_f1: 17.01</t>
+          <t>Epoch:109, time:11.945087, test_Acc: 30.00, test_bacc: 28.30, test_f1: 18.00</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>Epoch:99, time:11.973254, test_Acc: 29.40, test_bacc: 27.83, test_f1: 17.01</t>
+          <t>Epoch:108, time:11.341464, test_Acc: 30.00, test_bacc: 28.30, test_f1: 18.00</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>Epoch:98, time:11.007429, test_Acc: 29.40, test_bacc: 27.83, test_f1: 17.01</t>
+          <t>Epoch:107, time:11.205988, test_Acc: 30.00, test_bacc: 28.30, test_f1: 18.00</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>Epoch:97, time:12.100090, test_Acc: 29.40, test_bacc: 27.83, test_f1: 17.01</t>
+          <t>Epoch:106, time:11.058895, test_Acc: 29.90, test_bacc: 28.25, test_f1: 17.60</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>Epoch:96, time:11.237657, test_Acc: 28.90, test_bacc: 27.34, test_f1: 16.67</t>
+          <t>Epoch:105, time:11.460838, test_Acc: 29.90, test_bacc: 28.25, test_f1: 17.60</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>Epoch:95, time:12.380964, test_Acc: 28.90, test_bacc: 27.34, test_f1: 16.67</t>
+          <t>Epoch:104, time:11.180882, test_Acc: 29.90, test_bacc: 28.25, test_f1: 17.60</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>Epoch:94, time:11.442470, test_Acc: 28.90, test_bacc: 27.34, test_f1: 16.67</t>
+          <t>Epoch:103, time:10.792564, test_Acc: 29.90, test_bacc: 28.25, test_f1: 17.60</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>Epoch:93, time:10.915231, test_Acc: 28.90, test_bacc: 27.34, test_f1: 16.67</t>
+          <t>Epoch:102, time:11.128788, test_Acc: 29.80, test_bacc: 28.15, test_f1: 17.64</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>Epoch:92, time:11.880943, test_Acc: 28.50, test_bacc: 26.94, test_f1: 16.50</t>
+          <t>Epoch:101, time:13.083462, test_Acc: 29.80, test_bacc: 28.15, test_f1: 17.64</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>Epoch:91, time:11.936515, test_Acc: 28.50, test_bacc: 26.94, test_f1: 16.50</t>
+          <t>Epoch:100, time:11.609606, test_Acc: 29.40, test_bacc: 27.83, test_f1: 17.01</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>Epoch:90, time:11.251738, test_Acc: 28.20, test_bacc: 26.64, test_f1: 16.49</t>
+          <t>Epoch:99, time:11.973254, test_Acc: 29.40, test_bacc: 27.83, test_f1: 17.01</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>Epoch:89, time:10.508940, test_Acc: 28.20, test_bacc: 26.64, test_f1: 16.49</t>
+          <t>Epoch:98, time:11.007429, test_Acc: 29.40, test_bacc: 27.83, test_f1: 17.01</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>Epoch:88, time:12.314361, test_Acc: 27.70, test_bacc: 26.15, test_f1: 16.25</t>
+          <t>Epoch:97, time:12.100090, test_Acc: 29.40, test_bacc: 27.83, test_f1: 17.01</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>Epoch:87, time:10.574090, test_Acc: 27.70, test_bacc: 26.15, test_f1: 16.25</t>
+          <t>Epoch:96, time:11.237657, test_Acc: 28.90, test_bacc: 27.34, test_f1: 16.67</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>Epoch:86, time:11.746787, test_Acc: 27.30, test_bacc: 25.75, test_f1: 16.11</t>
+          <t>Epoch:95, time:12.380964, test_Acc: 28.90, test_bacc: 27.34, test_f1: 16.67</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>Epoch:85, time:10.426637, test_Acc: 27.30, test_bacc: 25.75, test_f1: 16.11</t>
+          <t>Epoch:94, time:11.442470, test_Acc: 28.90, test_bacc: 27.34, test_f1: 16.67</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>Epoch:84, time:11.048239, test_Acc: 26.80, test_bacc: 25.25, test_f1: 15.80</t>
+          <t>Epoch:93, time:10.915231, test_Acc: 28.90, test_bacc: 27.34, test_f1: 16.67</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>Epoch:83, time:11.162655, test_Acc: 26.80, test_bacc: 25.25, test_f1: 15.80</t>
+          <t>Epoch:92, time:11.880943, test_Acc: 28.50, test_bacc: 26.94, test_f1: 16.50</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>Epoch:82, time:10.641183, test_Acc: 26.60, test_bacc: 25.06, test_f1: 15.69</t>
+          <t>Epoch:91, time:11.936515, test_Acc: 28.50, test_bacc: 26.94, test_f1: 16.50</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>Epoch:81, time:12.131608, test_Acc: 26.60, test_bacc: 25.06, test_f1: 15.69</t>
+          <t>Epoch:90, time:11.251738, test_Acc: 28.20, test_bacc: 26.64, test_f1: 16.49</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>Epoch:80, time:11.527268, test_Acc: 26.20, test_bacc: 24.65, test_f1: 15.43</t>
+          <t>Epoch:89, time:10.508940, test_Acc: 28.20, test_bacc: 26.64, test_f1: 16.49</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>Epoch:79, time:11.235849, test_Acc: 26.20, test_bacc: 24.65, test_f1: 15.43</t>
+          <t>Epoch:88, time:12.314361, test_Acc: 27.70, test_bacc: 26.15, test_f1: 16.25</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>Epoch:78, time:11.181425, test_Acc: 25.80, test_bacc: 24.26, test_f1: 15.06</t>
+          <t>Epoch:87, time:10.574090, test_Acc: 27.70, test_bacc: 26.15, test_f1: 16.25</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>Epoch:77, time:12.115339, test_Acc: 25.80, test_bacc: 24.26, test_f1: 15.06</t>
+          <t>Epoch:86, time:11.746787, test_Acc: 27.30, test_bacc: 25.75, test_f1: 16.11</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>Epoch:76, time:12.025380, test_Acc: 25.20, test_bacc: 23.67, test_f1: 14.52</t>
+          <t>Epoch:85, time:10.426637, test_Acc: 27.30, test_bacc: 25.75, test_f1: 16.11</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>Epoch:75, time:11.456558, test_Acc: 25.20, test_bacc: 23.67, test_f1: 14.52</t>
+          <t>Epoch:84, time:11.048239, test_Acc: 26.80, test_bacc: 25.25, test_f1: 15.80</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>Epoch:74, time:12.290942, test_Acc: 25.10, test_bacc: 23.57, test_f1: 14.54</t>
+          <t>Epoch:83, time:11.162655, test_Acc: 26.80, test_bacc: 25.25, test_f1: 15.80</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>Epoch:73, time:11.965064, test_Acc: 25.10, test_bacc: 23.57, test_f1: 14.54</t>
+          <t>Epoch:82, time:10.641183, test_Acc: 26.60, test_bacc: 25.06, test_f1: 15.69</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>Epoch:72, time:10.636973, test_Acc: 24.30, test_bacc: 22.78, test_f1: 13.84</t>
+          <t>Epoch:81, time:12.131608, test_Acc: 26.60, test_bacc: 25.06, test_f1: 15.69</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>Epoch:71, time:10.832816, test_Acc: 24.30, test_bacc: 22.78, test_f1: 13.84</t>
+          <t>Epoch:80, time:11.527268, test_Acc: 26.20, test_bacc: 24.65, test_f1: 15.43</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>Epoch:70, time:11.665779, test_Acc: 23.40, test_bacc: 21.89, test_f1: 13.07</t>
+          <t>Epoch:79, time:11.235849, test_Acc: 26.20, test_bacc: 24.65, test_f1: 15.43</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>Epoch:69, time:11.233691, test_Acc: 21.70, test_bacc: 20.22, test_f1: 11.01</t>
+          <t>Epoch:78, time:11.181425, test_Acc: 25.80, test_bacc: 24.26, test_f1: 15.06</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>Epoch:68, time:10.882602, test_Acc: 21.70, test_bacc: 20.22, test_f1: 11.01</t>
+          <t>Epoch:77, time:12.115339, test_Acc: 25.80, test_bacc: 24.26, test_f1: 15.06</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>Epoch:67, time:11.622828, test_Acc: 20.60, test_bacc: 19.13, test_f1: 9.45</t>
+          <t>Epoch:76, time:12.025380, test_Acc: 25.20, test_bacc: 23.67, test_f1: 14.52</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>Epoch:66, time:11.727852, test_Acc: 20.40, test_bacc: 18.93, test_f1: 9.14</t>
+          <t>Epoch:75, time:11.456558, test_Acc: 25.20, test_bacc: 23.67, test_f1: 14.52</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>Epoch:65, time:11.736851, test_Acc: 20.40, test_bacc: 18.93, test_f1: 9.14</t>
+          <t>Epoch:74, time:12.290942, test_Acc: 25.10, test_bacc: 23.57, test_f1: 14.54</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>Epoch:64, time:11.114628, test_Acc: 19.70, test_bacc: 18.24, test_f1: 8.03</t>
+          <t>Epoch:73, time:11.965064, test_Acc: 25.10, test_bacc: 23.57, test_f1: 14.54</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>Epoch:63, time:11.429907, test_Acc: 19.70, test_bacc: 18.24, test_f1: 8.03</t>
+          <t>Epoch:72, time:10.636973, test_Acc: 24.30, test_bacc: 22.78, test_f1: 13.84</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>Epoch:62, time:11.619343, test_Acc: 19.00, test_bacc: 17.55, test_f1: 6.83</t>
+          <t>Epoch:71, time:10.832816, test_Acc: 24.30, test_bacc: 22.78, test_f1: 13.84</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>Epoch:61, time:11.048489, test_Acc: 19.00, test_bacc: 17.55, test_f1: 6.83</t>
+          <t>Epoch:70, time:11.665779, test_Acc: 23.40, test_bacc: 21.89, test_f1: 13.07</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>Epoch:60, time:11.300883, test_Acc: 18.90, test_bacc: 17.46, test_f1: 6.65</t>
+          <t>Epoch:69, time:11.233691, test_Acc: 21.70, test_bacc: 20.22, test_f1: 11.01</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>Epoch:59, time:11.100424, test_Acc: 18.40, test_bacc: 16.96, test_f1: 5.70</t>
+          <t>Epoch:68, time:10.882602, test_Acc: 21.70, test_bacc: 20.22, test_f1: 11.01</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>Epoch:58, time:11.352797, test_Acc: 18.40, test_bacc: 16.96, test_f1: 5.70</t>
+          <t>Epoch:67, time:11.622828, test_Acc: 20.60, test_bacc: 19.13, test_f1: 9.45</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>Epoch:57, time:11.404162, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:66, time:11.727852, test_Acc: 20.40, test_bacc: 18.93, test_f1: 9.14</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>Epoch:56, time:11.358164, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:65, time:11.736851, test_Acc: 20.40, test_bacc: 18.93, test_f1: 9.14</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>Epoch:55, time:10.550078, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:64, time:11.114628, test_Acc: 19.70, test_bacc: 18.24, test_f1: 8.03</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>Epoch:54, time:11.575114, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:63, time:11.429907, test_Acc: 19.70, test_bacc: 18.24, test_f1: 8.03</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>Epoch:53, time:10.337696, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:62, time:11.619343, test_Acc: 19.00, test_bacc: 17.55, test_f1: 6.83</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>Epoch:52, time:10.689744, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:61, time:11.048489, test_Acc: 19.00, test_bacc: 17.55, test_f1: 6.83</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>Epoch:51, time:12.427894, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:60, time:11.300883, test_Acc: 18.90, test_bacc: 17.46, test_f1: 6.65</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>Epoch:50, time:11.589657, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:59, time:11.100424, test_Acc: 18.40, test_bacc: 16.96, test_f1: 5.70</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>Epoch:49, time:9.989787, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:58, time:11.352797, test_Acc: 18.40, test_bacc: 16.96, test_f1: 5.70</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>Epoch:48, time:9.442720, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:57, time:11.404162, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>Epoch:47, time:9.992970, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:56, time:11.358164, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>Epoch:46, time:9.490592, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:55, time:10.550078, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>Epoch:45, time:10.073120, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:54, time:11.575114, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>Epoch:44, time:9.976090, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:53, time:10.337696, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>Epoch:43, time:9.358679, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:52, time:10.689744, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>Epoch:42, time:9.222989, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:51, time:12.427894, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>Epoch:41, time:9.525244, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:50, time:11.589657, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>Epoch:40, time:9.654254, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:49, time:9.989787, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>Epoch:39, time:9.035968, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:48, time:9.442720, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>Epoch:38, time:9.049059, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:47, time:9.992970, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>Epoch:37, time:8.958759, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:46, time:9.490592, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>Epoch:36, time:9.001986, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:45, time:10.073120, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>Epoch:35, time:9.474865, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:44, time:9.976090, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>Epoch:34, time:9.028265, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:43, time:9.358679, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>Epoch:33, time:8.953489, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:42, time:9.222989, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>Epoch:32, time:9.107829, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:41, time:9.525244, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>Epoch:31, time:9.002049, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:40, time:9.654254, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>Epoch:30, time:8.895467, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:39, time:9.035968, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>Epoch:29, time:9.041481, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:38, time:9.049059, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>Epoch:28, time:9.391772, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:37, time:8.958759, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>Epoch:27, time:9.702795, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:36, time:9.001986, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>Epoch:26, time:9.365391, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:35, time:9.474865, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>Epoch:25, time:9.077323, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:34, time:9.028265, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>Epoch:24, time:9.171938, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:33, time:8.953489, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>Epoch:23, time:9.153638, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:32, time:9.107829, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>Epoch:22, time:9.446651, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:31, time:9.002049, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>Epoch:21, time:9.716231, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:30, time:8.895467, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>Epoch:20, time:9.031900, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:29, time:9.041481, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>Epoch:19, time:9.589604, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:28, time:9.391772, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>Epoch:18, time:9.848087, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:27, time:9.702795, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>Epoch:17, time:9.416550, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:26, time:9.365391, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>Epoch:16, time:9.226005, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:25, time:9.077323, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>Epoch:15, time:8.975170, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:24, time:9.171938, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>Epoch:14, time:9.198755, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:23, time:9.153638, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>Epoch:13, time:9.117274, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:22, time:9.446651, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>Epoch:12, time:9.230316, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:21, time:9.716231, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>Epoch:11, time:9.146341, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:20, time:9.031900, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>Epoch:10, time:9.066450, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:19, time:9.589604, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>Epoch:9, time:9.032682, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:18, time:9.848087, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>Epoch:8, time:8.980339, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:17, time:9.416550, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>Epoch:7, time:8.987084, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:16, time:9.226005, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>Epoch:6, time:9.221040, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:15, time:8.975170, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>Epoch:5, time:17.831537, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:14, time:9.198755, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>Epoch:4, time:18.361759, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:13, time:9.117274, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>Epoch:3, time:18.394424, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:12, time:9.230316, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>Epoch:2, time:18.315672, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:11, time:9.146341, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>Epoch:1, time:17.575878, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+          <t>Epoch:10, time:9.066450, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
         </is>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
+        <is>
+          <t>Epoch:9, time:9.032682, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>Epoch:8, time:8.980339, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>Epoch:7, time:8.987084, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>Epoch:6, time:9.221040, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>Epoch:5, time:17.831537, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>Epoch:4, time:18.361759, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>Epoch:3, time:18.394424, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>Epoch:2, time:18.315672, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>Epoch:1, time:17.575878, test_Acc: 18.10, test_bacc: 16.67, test_f1: 5.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
         <is>
           <t>Epoch:0, time:19.058688, test_Acc: 17.00, test_bacc: 16.76, test_f1: 5.01</t>
         </is>

</xml_diff>